<commit_message>
profiles of clusters (approximately)
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/median of clusters-2.xlsx
+++ b/migforecasting/clustering/median of clusters-2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="41">
   <si>
     <t>clust</t>
   </si>
@@ -126,6 +126,24 @@
   <si>
     <t>Вектор развития согласно сценарию</t>
   </si>
+  <si>
+    <t>profile</t>
+  </si>
+  <si>
+    <t>сельхоз (посев)</t>
+  </si>
+  <si>
+    <t>сельхоз (скот, худший)</t>
+  </si>
+  <si>
+    <t>сельхоз (скот)</t>
+  </si>
+  <si>
+    <t>гибрид лучший</t>
+  </si>
+  <si>
+    <t>гибрид средний</t>
+  </si>
 </sst>
 </file>
 
@@ -184,7 +202,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,8 +215,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -232,11 +256,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -272,6 +305,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -304,7 +346,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -549,7 +590,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -797,7 +837,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1045,7 +1084,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1290,7 +1328,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1535,7 +1572,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1780,7 +1816,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2028,7 +2063,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3058,7 +3092,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3397,7 +3430,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3675,7 +3707,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4430,7 +4461,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4786,7 +4816,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5034,7 +5063,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5279,7 +5307,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5527,7 +5554,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5775,7 +5801,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6023,7 +6048,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6271,7 +6295,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19489,7 +19512,7 @@
   <dimension ref="A1:AB27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="O3" sqref="M3:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21851,7 +21874,7 @@
   <dimension ref="A1:AR22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21859,7 +21882,8 @@
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="15.140625" customWidth="1"/>
     <col min="7" max="7" width="13.140625" customWidth="1"/>
-    <col min="19" max="19" width="11.28515625" customWidth="1"/>
+    <col min="19" max="19" width="23.140625" customWidth="1"/>
+    <col min="20" max="20" width="24.140625" customWidth="1"/>
     <col min="27" max="27" width="17.28515625" customWidth="1"/>
     <col min="29" max="29" width="12.85546875" customWidth="1"/>
   </cols>
@@ -21924,8 +21948,11 @@
       <c r="R2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="15" t="s">
         <v>27</v>
+      </c>
+      <c r="T2" s="16" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -21988,6 +22015,9 @@
         <f t="shared" ref="S3:S8" si="1">ABS(R3-B3)</f>
         <v>103.3633601576628</v>
       </c>
+      <c r="T3" s="17" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -22049,6 +22079,9 @@
         <f t="shared" si="1"/>
         <v>69.083100673347985</v>
       </c>
+      <c r="T4" s="17" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -22110,6 +22143,9 @@
         <f t="shared" si="1"/>
         <v>253.48382328790021</v>
       </c>
+      <c r="T5" s="17" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -22171,6 +22207,9 @@
         <f t="shared" si="1"/>
         <v>5.0042699950743668</v>
       </c>
+      <c r="T6" s="17" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -22232,6 +22271,9 @@
         <f t="shared" si="1"/>
         <v>96.36627525045418</v>
       </c>
+      <c r="T7" s="17" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -22291,6 +22333,9 @@
       <c r="S8" s="6">
         <f t="shared" si="1"/>
         <v>9.9475983006414026E-14</v>
+      </c>
+      <c r="T8" s="17" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>